<commit_message>
Added support to alter cell width and height
</commit_message>
<xml_diff>
--- a/RectangleDetectorOutput/test.xlsx
+++ b/RectangleDetectorOutput/test.xlsx
@@ -14,153 +14,114 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="36">
-  <si>
-    <t xml:space="preserve">Visual Inspection Notes: Wh ay Jl-/- 992z-l ' FIN -WOww
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">60
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Several
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">11-1-7729
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">| Go/no go |
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Glue - Spreader bar - Check for
-"WW" thread
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Glue - Riser Set - 11R - Check for
-Thread presents
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1/2
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Riser Set Offset
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C1
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1/4
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AQ
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">48 1/2
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">47 1/2
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Overall Length
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bottom Left
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Drawing
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Inspection Date: Qizlex |
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Te
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">T11R Risers
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Visual Inspection + Canopy Release Functional w/ Harness (GO/NO GO) : '
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Car
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">B2/B5
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">11-1-7719
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Go/No-Go
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Glue - Riser set - Check thread
-presents
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">G4
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Riser Leg Offset
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">26
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">28 1/4
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Overall Length
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Inspection Date: Q
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DoM: §$)z=
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">T11 Risers
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Box #1
-</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="35">
+  <si>
+    <t>Visual Inspection Notes: Wh ay Jl-/- 992z-l ' FIN -WOww</t>
+  </si>
+  <si>
+    <t>60</t>
+  </si>
+  <si>
+    <t>Several</t>
+  </si>
+  <si>
+    <t>11-1-7729</t>
+  </si>
+  <si>
+    <t>| Go/no go |</t>
+  </si>
+  <si>
+    <t>Glue - Spreader bar - Check for
+"WW" thread</t>
+  </si>
+  <si>
+    <t>Glue - Riser Set - 11R - Check for
+Thread presents</t>
+  </si>
+  <si>
+    <t>1/2</t>
+  </si>
+  <si>
+    <t>Riser Set Offset</t>
+  </si>
+  <si>
+    <t>C1</t>
+  </si>
+  <si>
+    <t>1/4</t>
+  </si>
+  <si>
+    <t>AQ</t>
+  </si>
+  <si>
+    <t>48 1/2</t>
+  </si>
+  <si>
+    <t>47 1/2</t>
+  </si>
+  <si>
+    <t>Overall Length</t>
+  </si>
+  <si>
+    <t>Bottom Left</t>
+  </si>
+  <si>
+    <t>Drawing</t>
+  </si>
+  <si>
+    <t>Inspection Date: Qizlex |</t>
+  </si>
+  <si>
+    <t>Te</t>
+  </si>
+  <si>
+    <t>T11R Risers</t>
+  </si>
+  <si>
+    <t>Visual Inspection + Canopy Release Functional w/ Harness (GO/NO GO) : '</t>
+  </si>
+  <si>
+    <t>Car</t>
+  </si>
+  <si>
+    <t>B2/B5</t>
+  </si>
+  <si>
+    <t>11-1-7719</t>
+  </si>
+  <si>
+    <t>Go/No-Go</t>
+  </si>
+  <si>
+    <t>Glue - Riser set - Check thread
+presents</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>G4</t>
+  </si>
+  <si>
+    <t>Riser Leg Offset</t>
+  </si>
+  <si>
+    <t>26</t>
+  </si>
+  <si>
+    <t>28 1/4</t>
+  </si>
+  <si>
+    <t>Inspection Date: Q</t>
+  </si>
+  <si>
+    <t>DoM: §$)z=</t>
+  </si>
+  <si>
+    <t>T11 Risers</t>
+  </si>
+  <si>
+    <t>Box #1</t>
   </si>
 </sst>
 </file>
@@ -390,88 +351,88 @@
   <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="20" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="21" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="22" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="23" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="24" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="25" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="26" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="28" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="29" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -767,34 +728,46 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:L19"/>
+  <dimension ref="A2:L19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="5.5703125" customWidth="1"/>
+    <col min="3" max="3" width="28.140625" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" customWidth="1"/>
+    <col min="5" max="5" width="8.5703125" customWidth="1"/>
+    <col min="6" max="6" width="9.42578125" customWidth="1"/>
+    <col min="7" max="7" width="6" customWidth="1"/>
+    <col min="8" max="8" width="8.28515625" customWidth="1"/>
+    <col min="9" max="9" width="8.140625" customWidth="1"/>
+    <col min="10" max="10" width="11.7109375" customWidth="1"/>
+    <col min="11" max="11" width="9" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="2:12">
+    <row r="2" spans="2:12" ht="16" customHeight="1">
       <c r="B2" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
       <c r="G2" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
       <c r="J2" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="K2" s="4"/>
       <c r="L2" s="3"/>
     </row>
-    <row r="3" spans="2:12">
+    <row r="3" spans="2:12" ht="17.25" customHeight="1">
       <c r="B3" s="5"/>
       <c r="C3" s="6"/>
       <c r="D3" s="1"/>
@@ -808,10 +781,10 @@
       </c>
       <c r="K3" s="9"/>
     </row>
-    <row r="4" spans="2:12">
+    <row r="4" spans="2:12" ht="22.5" customHeight="1">
       <c r="B4" s="10"/>
       <c r="C4" s="3" t="s">
-        <v>31</v>
+        <v>14</v>
       </c>
       <c r="D4" s="3"/>
       <c r="E4" s="1" t="s">
@@ -829,7 +802,7 @@
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
     </row>
-    <row r="5" spans="2:12">
+    <row r="5" spans="2:12" ht="22.25" customHeight="1">
       <c r="B5" s="11"/>
       <c r="C5" s="1" t="s">
         <v>28</v>
@@ -848,7 +821,7 @@
       <c r="K5" s="1"/>
       <c r="L5" s="12"/>
     </row>
-    <row r="6" spans="2:12">
+    <row r="6" spans="2:12" ht="26" customHeight="1">
       <c r="B6" s="13" t="s">
         <v>26</v>
       </c>
@@ -873,7 +846,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="2:12">
+    <row r="7" spans="2:12" ht="16.25" customHeight="1">
       <c r="B7" s="14" t="s">
         <v>20</v>
       </c>
@@ -888,7 +861,7 @@
       <c r="K7" s="16"/>
       <c r="L7" s="12"/>
     </row>
-    <row r="8" spans="2:12">
+    <row r="8" spans="2:12" ht="17.75" customHeight="1">
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
@@ -901,7 +874,8 @@
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
     </row>
-    <row r="10" spans="2:12">
+    <row r="9" spans="2:12" ht="78.25" customHeight="1"/>
+    <row r="10" spans="2:12" ht="16.75" customHeight="1">
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="3" t="s">
@@ -920,7 +894,7 @@
       <c r="K10" s="7"/>
       <c r="L10" s="7"/>
     </row>
-    <row r="11" spans="2:12">
+    <row r="11" spans="2:12" ht="16.5" customHeight="1">
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="2"/>
@@ -936,7 +910,7 @@
       </c>
       <c r="K11" s="17"/>
     </row>
-    <row r="12" spans="2:12">
+    <row r="12" spans="2:12" ht="22.5" customHeight="1">
       <c r="B12" s="18"/>
       <c r="C12" s="1" t="s">
         <v>14</v>
@@ -959,7 +933,7 @@
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
     </row>
-    <row r="13" spans="2:12">
+    <row r="13" spans="2:12" ht="23.5" customHeight="1">
       <c r="B13" s="19"/>
       <c r="C13" s="2"/>
       <c r="D13" s="1"/>
@@ -978,7 +952,7 @@
       <c r="K13" s="1"/>
       <c r="L13" s="22"/>
     </row>
-    <row r="14" spans="2:12">
+    <row r="14" spans="2:12" ht="21.25" customHeight="1">
       <c r="B14" s="18"/>
       <c r="C14" s="1" t="s">
         <v>8</v>
@@ -997,7 +971,7 @@
       <c r="K14" s="22"/>
       <c r="L14" s="22"/>
     </row>
-    <row r="15" spans="2:12">
+    <row r="15" spans="2:12" ht="28.5" customHeight="1">
       <c r="B15" s="18"/>
       <c r="C15" s="3" t="s">
         <v>6</v>
@@ -1018,7 +992,7 @@
       <c r="K15" s="23"/>
       <c r="L15" s="21"/>
     </row>
-    <row r="16" spans="2:12">
+    <row r="16" spans="2:12" ht="30.25" customHeight="1">
       <c r="B16" s="19"/>
       <c r="C16" s="3" t="s">
         <v>5</v>
@@ -1041,7 +1015,7 @@
       <c r="K16" s="21"/>
       <c r="L16" s="22"/>
     </row>
-    <row r="17" spans="2:12">
+    <row r="17" spans="2:12" ht="16" customHeight="1">
       <c r="B17" s="25"/>
       <c r="C17" s="25"/>
       <c r="D17" s="25"/>
@@ -1054,7 +1028,7 @@
       <c r="K17" s="22"/>
       <c r="L17" s="28"/>
     </row>
-    <row r="18" spans="2:12">
+    <row r="18" spans="2:12" ht="17.75" customHeight="1">
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>

</xml_diff>